<commit_message>
add IEEE 69 bus in flow analysis
</commit_message>
<xml_diff>
--- a/ieee33_results.xlsx
+++ b/ieee33_results.xlsx
@@ -473,10 +473,10 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>-3.917677069368892</v>
+        <v>-3.917677035742884</v>
       </c>
       <c r="E2" t="n">
-        <v>-2.435140928377848</v>
+        <v>-2.435140909341271</v>
       </c>
     </row>
     <row r="3">
@@ -484,10 +484,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.9970322597745299</v>
+        <v>0.9970322597994554</v>
       </c>
       <c r="C3" t="n">
-        <v>0.01448141361819512</v>
+        <v>0.01448141355517385</v>
       </c>
       <c r="D3" t="n">
         <v>0.1</v>
@@ -501,10 +501,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.982937983682625</v>
+        <v>0.982937983840579</v>
       </c>
       <c r="C4" t="n">
-        <v>0.09604157808731982</v>
+        <v>0.09604157751759158</v>
       </c>
       <c r="D4" t="n">
         <v>0.09</v>
@@ -518,10 +518,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.975456413684887</v>
+        <v>0.9754564139398851</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1616514426420938</v>
+        <v>0.161651441249463</v>
       </c>
       <c r="D5" t="n">
         <v>0.12</v>
@@ -535,10 +535,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.9680592330026594</v>
+        <v>0.9680592333565587</v>
       </c>
       <c r="C6" t="n">
-        <v>0.2282853545469826</v>
+        <v>0.2282853515253835</v>
       </c>
       <c r="D6" t="n">
         <v>0.06</v>
@@ -552,10 +552,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.9496581785143297</v>
+        <v>0.9496581791054797</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1338532552743818</v>
+        <v>0.133853245117732</v>
       </c>
       <c r="D7" t="n">
         <v>0.06</v>
@@ -569,10 +569,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>0.9461726147190664</v>
+        <v>0.9461726153119692</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.09647402888056171</v>
+        <v>-0.09647404570143439</v>
       </c>
       <c r="D8" t="n">
         <v>0.2</v>
@@ -586,10 +586,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0.9413284385480489</v>
+        <v>0.9413284391615621</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.06040303044120004</v>
+        <v>-0.0604030519488914</v>
       </c>
       <c r="D9" t="n">
         <v>0.2000000000000001</v>
@@ -603,10 +603,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>0.9350593736954195</v>
+        <v>0.9350593743306729</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.1334844732622515</v>
+        <v>-0.1334845066882773</v>
       </c>
       <c r="D10" t="n">
         <v>0.06000000000000005</v>
@@ -620,10 +620,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>0.9292444242853557</v>
+        <v>0.9292444249373505</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.1960140185432623</v>
+        <v>-0.1960140670832908</v>
       </c>
       <c r="D11" t="n">
         <v>0.06000000000000005</v>
@@ -637,10 +637,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>0.9283844188825485</v>
+        <v>0.9283844195367964</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.1887610561347207</v>
+        <v>-0.1887611063456613</v>
       </c>
       <c r="D12" t="n">
         <v>0.04500000000000004</v>
@@ -654,10 +654,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>0.9268848385130563</v>
+        <v>0.9268848391700895</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.1772689535117754</v>
+        <v>-0.1772690067667021</v>
       </c>
       <c r="D13" t="n">
         <v>0.05999999999999994</v>
@@ -671,10 +671,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>0.9207717495299219</v>
+        <v>0.9207717501890819</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.2685864988710654</v>
+        <v>-0.268586577719308</v>
       </c>
       <c r="D14" t="n">
         <v>0.06000000000000005</v>
@@ -688,10 +688,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>0.9185049948260666</v>
+        <v>0.9185049954866683</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.347267455358653</v>
+        <v>-0.3472675501159292</v>
       </c>
       <c r="D15" t="n">
         <v>0.1200000000000001</v>
@@ -705,10 +705,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>0.9170926822244143</v>
+        <v>0.9170926828880497</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.3849502047257227</v>
+        <v>-0.3849503083249661</v>
       </c>
       <c r="D16" t="n">
         <v>0.06000000000000005</v>
@@ -722,10 +722,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>0.9157247622342469</v>
+        <v>0.9157247629013583</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.4082048824020456</v>
+        <v>-0.4082049937800342</v>
       </c>
       <c r="D17" t="n">
         <v>0.06000000000000005</v>
@@ -739,10 +739,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>0.91369754838413</v>
+        <v>0.9136975490580841</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.485473106118393</v>
+        <v>-0.4854732356795773</v>
       </c>
       <c r="D18" t="n">
         <v>0.06000000000000005</v>
@@ -756,10 +756,10 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>0.9130904816081867</v>
+        <v>0.9130904822858236</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.4950626717676198</v>
+        <v>-0.4950628054058378</v>
       </c>
       <c r="D19" t="n">
         <v>0.09000000000000008</v>
@@ -773,10 +773,10 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>0.9965038957000354</v>
+        <v>0.9965038957249749</v>
       </c>
       <c r="C20" t="n">
-        <v>0.003650895266597073</v>
+        <v>0.003650895204048404</v>
       </c>
       <c r="D20" t="n">
         <v>0.09000000000000008</v>
@@ -790,10 +790,10 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>0.9929262995769307</v>
+        <v>0.9929262996019639</v>
       </c>
       <c r="C21" t="n">
-        <v>-0.06332768339004395</v>
+        <v>-0.06332768345022945</v>
       </c>
       <c r="D21" t="n">
         <v>0.09000000000000008</v>
@@ -807,10 +807,10 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>0.9922217958661075</v>
+        <v>0.992221795891159</v>
       </c>
       <c r="C22" t="n">
-        <v>-0.0826855621824885</v>
+        <v>-0.08268556224204045</v>
       </c>
       <c r="D22" t="n">
         <v>0.09000000000000008</v>
@@ -824,10 +824,10 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>0.9915843769033287</v>
+        <v>0.9915843769283971</v>
       </c>
       <c r="C23" t="n">
-        <v>-0.1030331332492532</v>
+        <v>-0.1030331333081366</v>
       </c>
       <c r="D23" t="n">
         <v>0.09000000000000008</v>
@@ -841,10 +841,10 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>0.9793522576251699</v>
+        <v>0.9793522577841847</v>
       </c>
       <c r="C24" t="n">
-        <v>0.06507995623052448</v>
+        <v>0.06507995555553145</v>
       </c>
       <c r="D24" t="n">
         <v>0.09000000000000008</v>
@@ -858,10 +858,10 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>0.9726811012625085</v>
+        <v>0.972681101423474</v>
       </c>
       <c r="C25" t="n">
-        <v>-0.02365392995510519</v>
+        <v>-0.02365393094730225</v>
       </c>
       <c r="D25" t="n">
         <v>0.4199999999999999</v>
@@ -875,10 +875,10 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>0.9693561127498278</v>
+        <v>0.9693561129117781</v>
       </c>
       <c r="C26" t="n">
-        <v>-0.06735454831023359</v>
+        <v>-0.06735454953277345</v>
       </c>
       <c r="D26" t="n">
         <v>0.4199999999999999</v>
@@ -892,10 +892,10 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>0.947728911303972</v>
+        <v>0.9477289119405536</v>
       </c>
       <c r="C27" t="n">
-        <v>0.1733096050721166</v>
+        <v>0.1733095923453239</v>
       </c>
       <c r="D27" t="n">
         <v>0.06000000000000005</v>
@@ -909,10 +909,10 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>0.9451651654770823</v>
+        <v>0.945165166174232</v>
       </c>
       <c r="C28" t="n">
-        <v>0.2294631452743454</v>
+        <v>0.2294631285985286</v>
       </c>
       <c r="D28" t="n">
         <v>0.06000000000000005</v>
@@ -926,10 +926,10 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>0.9337255824795435</v>
+        <v>0.9337255834143975</v>
       </c>
       <c r="C29" t="n">
-        <v>0.3124091097476208</v>
+        <v>0.312409071732868</v>
       </c>
       <c r="D29" t="n">
         <v>0.06000000000000005</v>
@@ -943,10 +943,10 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>0.9255074801591789</v>
+        <v>0.9255074812208577</v>
       </c>
       <c r="C30" t="n">
-        <v>0.3903144187759809</v>
+        <v>0.3903143551029033</v>
       </c>
       <c r="D30" t="n">
         <v>0.1200000000000001</v>
@@ -960,10 +960,10 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>0.9219500597738733</v>
+        <v>0.9219500608719307</v>
       </c>
       <c r="C31" t="n">
-        <v>0.4955855515830908</v>
+        <v>0.4955854737060638</v>
       </c>
       <c r="D31" t="n">
         <v>0.2000000000000002</v>
@@ -977,10 +977,10 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>0.9177888891110744</v>
+        <v>0.917788890239587</v>
       </c>
       <c r="C32" t="n">
-        <v>0.411177666877219</v>
+        <v>0.4111775645154899</v>
       </c>
       <c r="D32" t="n">
         <v>0.1499999999999999</v>
@@ -994,10 +994,10 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>0.916873467783712</v>
+        <v>0.9168734689196797</v>
       </c>
       <c r="C33" t="n">
-        <v>0.3881349380419881</v>
+        <v>0.3881348292268729</v>
       </c>
       <c r="D33" t="n">
         <v>0.21</v>
@@ -1011,10 +1011,10 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>0.9165898241911655</v>
+        <v>0.9165898253295394</v>
       </c>
       <c r="C34" t="n">
-        <v>0.3804050459193769</v>
+        <v>0.3804049349616199</v>
       </c>
       <c r="D34" t="n">
         <v>0.06000000000000005</v>
@@ -1087,19 +1087,19 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>3.917677069368892</v>
+        <v>3.917677035742884</v>
       </c>
       <c r="D2" t="n">
-        <v>2.435140928377848</v>
+        <v>2.435140909341271</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0002103664525176749</v>
+        <v>0.0002103664507569586</v>
       </c>
       <c r="F2" t="n">
-        <v>0.01224042385364221</v>
+        <v>0.01224042364874345</v>
       </c>
       <c r="G2" t="n">
-        <v>0.006239695456845329</v>
+        <v>0.006239695352396435</v>
       </c>
     </row>
     <row r="3">
@@ -1110,19 +1110,19 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>3.444299122859893</v>
+        <v>3.44429908981525</v>
       </c>
       <c r="D3" t="n">
-        <v>2.207822378826912</v>
+        <v>2.207822359262827</v>
       </c>
       <c r="E3" t="n">
-        <v>0.0001871321378675269</v>
+        <v>0.0001871321361074346</v>
       </c>
       <c r="F3" t="n">
-        <v>0.05179123251663853</v>
+        <v>0.05179123154238185</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0263788610241944</v>
+        <v>0.02637886052797578</v>
       </c>
     </row>
     <row r="4">
@@ -1133,19 +1133,19 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>2.362895135552793</v>
+        <v>2.362895105146355</v>
       </c>
       <c r="D4" t="n">
-        <v>1.684200469813067</v>
+        <v>1.684200448499956</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0001346278467357947</v>
+        <v>0.0001346278449914153</v>
       </c>
       <c r="F4" t="n">
-        <v>0.01990047549867446</v>
+        <v>0.01990047498297187</v>
       </c>
       <c r="G4" t="n">
-        <v>0.01013510555451647</v>
+        <v>0.01013510529187434</v>
       </c>
     </row>
     <row r="5">
@@ -1156,19 +1156,19 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>2.222994662189499</v>
+        <v>2.222994635041896</v>
       </c>
       <c r="D5" t="n">
-        <v>1.594065361064803</v>
+        <v>1.594065336236827</v>
       </c>
       <c r="E5" t="n">
-        <v>0.0001278888696325964</v>
+        <v>0.0001278888678913066</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0186989411659173</v>
+        <v>0.01869894065672106</v>
       </c>
       <c r="G5" t="n">
-        <v>0.009523653844934366</v>
+        <v>0.00952365358559315</v>
       </c>
     </row>
     <row r="6">
@@ -1179,19 +1179,19 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>2.144295716509867</v>
+        <v>2.144295702734075</v>
       </c>
       <c r="D6" t="n">
-        <v>1.554541714797618</v>
+        <v>1.55454168020865</v>
       </c>
       <c r="E6" t="n">
-        <v>0.0001247698519292763</v>
+        <v>0.0001247698504018268</v>
       </c>
       <c r="F6" t="n">
-        <v>0.03824862170635512</v>
+        <v>0.03824862076986602</v>
       </c>
       <c r="G6" t="n">
-        <v>0.03301804096018723</v>
+        <v>0.03301804015176435</v>
       </c>
     </row>
     <row r="7">
@@ -1202,19 +1202,19 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>1.095267324119346</v>
+        <v>1.095267350048974</v>
       </c>
       <c r="D7" t="n">
-        <v>0.5278877326624556</v>
+        <v>0.5278877250319957</v>
       </c>
       <c r="E7" t="n">
-        <v>5.838757736667102e-05</v>
+        <v>5.83875782929422e-05</v>
       </c>
       <c r="F7" t="n">
-        <v>0.00191451743060167</v>
+        <v>0.001914517491345968</v>
       </c>
       <c r="G7" t="n">
-        <v>0.006328543728933211</v>
+        <v>0.006328543929727592</v>
       </c>
     </row>
     <row r="8">
@@ -1225,19 +1225,19 @@
         <v>7</v>
       </c>
       <c r="C8" t="n">
-        <v>0.8933528437856385</v>
+        <v>0.8933528452411316</v>
       </c>
       <c r="D8" t="n">
-        <v>0.4215591745924244</v>
+        <v>0.4215591588206852</v>
       </c>
       <c r="E8" t="n">
-        <v>4.761218782511025e-05</v>
+        <v>4.761218753430568e-05</v>
       </c>
       <c r="F8" t="n">
-        <v>0.004837964819877527</v>
+        <v>0.004837964760778912</v>
       </c>
       <c r="G8" t="n">
-        <v>0.00159882700190217</v>
+        <v>0.001598826982371571</v>
       </c>
     </row>
     <row r="9">
@@ -1248,19 +1248,19 @@
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>0.6885148737140419</v>
+        <v>0.6885148856432253</v>
       </c>
       <c r="D9" t="n">
-        <v>0.3199603620400325</v>
+        <v>0.3199603418872784</v>
       </c>
       <c r="E9" t="n">
-        <v>3.678248998796069e-05</v>
+        <v>3.678249007663584e-05</v>
       </c>
       <c r="F9" t="n">
-        <v>0.004180536738428664</v>
+        <v>0.00418053675858554</v>
       </c>
       <c r="G9" t="n">
-        <v>0.003003492414016706</v>
+        <v>0.003003492428498289</v>
       </c>
     </row>
     <row r="10">
@@ -1271,19 +1271,19 @@
         <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>0.6243343369916093</v>
+        <v>0.6243343524909679</v>
       </c>
       <c r="D10" t="n">
-        <v>0.296956871328222</v>
+        <v>0.2969568469254671</v>
       </c>
       <c r="E10" t="n">
-        <v>3.371896275612098e-05</v>
+        <v>3.371896290465334e-05</v>
       </c>
       <c r="F10" t="n">
-        <v>0.00356091396401248</v>
+        <v>0.003560913995384274</v>
       </c>
       <c r="G10" t="n">
-        <v>0.002524019476407346</v>
+        <v>0.002524019498644003</v>
       </c>
     </row>
     <row r="11">
@@ -1294,19 +1294,19 @@
         <v>10</v>
       </c>
       <c r="C11" t="n">
-        <v>0.5607734322166823</v>
+        <v>0.5607734371634003</v>
       </c>
       <c r="D11" t="n">
-        <v>0.2744328357253498</v>
+        <v>0.2744328169756599</v>
       </c>
       <c r="E11" t="n">
-        <v>3.064008362290143e-05</v>
+        <v>3.064008341497948e-05</v>
       </c>
       <c r="F11" t="n">
-        <v>0.0005537018502589364</v>
+        <v>0.0005537018427441698</v>
       </c>
       <c r="G11" t="n">
-        <v>0.0001830652099025221</v>
+        <v>0.000183065207417954</v>
       </c>
     </row>
     <row r="12">
@@ -1317,19 +1317,19 @@
         <v>11</v>
       </c>
       <c r="C12" t="n">
-        <v>0.5152197308737526</v>
+        <v>0.5152197360534859</v>
       </c>
       <c r="D12" t="n">
-        <v>0.2442497717307923</v>
+        <v>0.2442497539773104</v>
       </c>
       <c r="E12" t="n">
-        <v>2.800895321282083e-05</v>
+        <v>2.800895304941615e-05</v>
       </c>
       <c r="F12" t="n">
-        <v>0.0008811344170068791</v>
+        <v>0.0008811344067256588</v>
       </c>
       <c r="G12" t="n">
-        <v>0.0002913580150253059</v>
+        <v>0.0002913580116256087</v>
       </c>
     </row>
     <row r="13">
@@ -1340,19 +1340,19 @@
         <v>12</v>
       </c>
       <c r="C13" t="n">
-        <v>0.4543385866127518</v>
+        <v>0.4543386071211826</v>
       </c>
       <c r="D13" t="n">
-        <v>0.2089584335219472</v>
+        <v>0.2089584078241144</v>
       </c>
       <c r="E13" t="n">
-        <v>2.460537253712954e-05</v>
+        <v>2.460537290811965e-05</v>
       </c>
       <c r="F13" t="n">
-        <v>0.002666235545760065</v>
+        <v>0.002666235626160918</v>
       </c>
       <c r="G13" t="n">
-        <v>0.002097753443700862</v>
+        <v>0.00209775350695901</v>
       </c>
     </row>
     <row r="14">
@@ -1363,19 +1363,19 @@
         <v>13</v>
       </c>
       <c r="C14" t="n">
-        <v>0.3916723372482926</v>
+        <v>0.3916723710136361</v>
       </c>
       <c r="D14" t="n">
-        <v>0.1718606895407405</v>
+        <v>0.1718606639989755</v>
       </c>
       <c r="E14" t="n">
-        <v>2.118440631880379e-05</v>
+        <v>2.118440732674837e-05</v>
       </c>
       <c r="F14" t="n">
-        <v>0.0007291616512393184</v>
+        <v>0.0007291617206257039</v>
       </c>
       <c r="G14" t="n">
-        <v>0.0009597846033392032</v>
+        <v>0.000959784694671395</v>
       </c>
     </row>
     <row r="15">
@@ -1386,19 +1386,19 @@
         <v>14</v>
       </c>
       <c r="C15" t="n">
-        <v>0.2709431909929834</v>
+        <v>0.270943208340841</v>
       </c>
       <c r="D15" t="n">
-        <v>0.09090090265304221</v>
+        <v>0.09090088262276716</v>
       </c>
       <c r="E15" t="n">
-        <v>1.418953744847063e-05</v>
+        <v>1.418953793853934e-05</v>
       </c>
       <c r="F15" t="n">
-        <v>0.0003569739515456583</v>
+        <v>0.0003569739762034896</v>
       </c>
       <c r="G15" t="n">
-        <v>0.0003177128570439891</v>
+        <v>0.0003177128789899064</v>
       </c>
     </row>
     <row r="16">
@@ -1409,19 +1409,19 @@
         <v>15</v>
       </c>
       <c r="C16" t="n">
-        <v>0.2105862245094676</v>
+        <v>0.2105862359093505</v>
       </c>
       <c r="D16" t="n">
-        <v>0.08058318515607293</v>
+        <v>0.08058316888868483</v>
       </c>
       <c r="E16" t="n">
-        <v>1.121244794590707e-05</v>
+        <v>1.121244817813679e-05</v>
       </c>
       <c r="F16" t="n">
-        <v>0.0002814666149203171</v>
+        <v>0.0002814666265796573</v>
       </c>
       <c r="G16" t="n">
-        <v>0.0002055464359259629</v>
+        <v>0.0002055464444404159</v>
       </c>
     </row>
     <row r="17">
@@ -1432,19 +1432,19 @@
         <v>16</v>
       </c>
       <c r="C17" t="n">
-        <v>0.1503047534515277</v>
+        <v>0.1503047691885276</v>
       </c>
       <c r="D17" t="n">
-        <v>0.06037764087963533</v>
+        <v>0.06037762866874647</v>
       </c>
       <c r="E17" t="n">
-        <v>8.066812468224607e-06</v>
+        <v>8.066812962917231e-06</v>
       </c>
       <c r="F17" t="n">
-        <v>0.0002516340502016767</v>
+        <v>0.000251634081064267</v>
       </c>
       <c r="G17" t="n">
-        <v>0.0003359675720690791</v>
+        <v>0.0003359676132751177</v>
       </c>
     </row>
     <row r="18">
@@ -1455,19 +1455,19 @@
         <v>17</v>
       </c>
       <c r="C18" t="n">
-        <v>0.0900531303726653</v>
+        <v>0.09005313630698146</v>
       </c>
       <c r="D18" t="n">
-        <v>0.04004166892003538</v>
+        <v>0.04004166052968241</v>
       </c>
       <c r="E18" t="n">
-        <v>4.919059134324488e-06</v>
+        <v>4.919059231195287e-06</v>
       </c>
       <c r="F18" t="n">
-        <v>5.313586278309079e-05</v>
+        <v>5.313586487588895e-05</v>
       </c>
       <c r="G18" t="n">
-        <v>4.166664649931512e-05</v>
+        <v>4.166664814039128e-05</v>
       </c>
     </row>
     <row r="19">
@@ -1478,19 +1478,19 @@
         <v>18</v>
       </c>
       <c r="C19" t="n">
-        <v>0.3611375234438792</v>
+        <v>0.3611375234441596</v>
       </c>
       <c r="D19" t="n">
-        <v>0.1610788528187309</v>
+        <v>0.1610788528180369</v>
       </c>
       <c r="E19" t="n">
-        <v>1.808726682940243e-05</v>
+        <v>1.808726682894903e-05</v>
       </c>
       <c r="F19" t="n">
-        <v>0.0001609541977759532</v>
+        <v>0.0001609541977677931</v>
       </c>
       <c r="G19" t="n">
-        <v>0.0001535934875117884</v>
+        <v>0.0001535934875041001</v>
       </c>
     </row>
     <row r="20">
@@ -1501,19 +1501,19 @@
         <v>19</v>
       </c>
       <c r="C20" t="n">
-        <v>0.2709765692461348</v>
+        <v>0.2709765692467913</v>
       </c>
       <c r="D20" t="n">
-        <v>0.1209252593314433</v>
+        <v>0.1209252593301995</v>
       </c>
       <c r="E20" t="n">
-        <v>1.357996643507662e-05</v>
+        <v>1.3579966434741e-05</v>
       </c>
       <c r="F20" t="n">
-        <v>0.0008321766890702631</v>
+        <v>0.0008321766890291293</v>
       </c>
       <c r="G20" t="n">
-        <v>0.0007498552615116394</v>
+        <v>0.0007498552614745857</v>
       </c>
     </row>
     <row r="21">
@@ -1524,19 +1524,19 @@
         <v>20</v>
       </c>
       <c r="C21" t="n">
-        <v>0.1801443925569811</v>
+        <v>0.1801443925580409</v>
       </c>
       <c r="D21" t="n">
-        <v>0.08017540407008091</v>
+        <v>0.08017540406902435</v>
       </c>
       <c r="E21" t="n">
-        <v>9.056422376822111e-06</v>
+        <v>9.05642237661853e-06</v>
       </c>
       <c r="F21" t="n">
-        <v>0.0001007580637379935</v>
+        <v>0.0001007580637334415</v>
       </c>
       <c r="G21" t="n">
-        <v>0.0001177110077955068</v>
+        <v>0.0001177110077902194</v>
       </c>
     </row>
     <row r="22">
@@ -1547,19 +1547,19 @@
         <v>21</v>
       </c>
       <c r="C22" t="n">
-        <v>0.09004363449376376</v>
+        <v>0.09004363449434934</v>
       </c>
       <c r="D22" t="n">
-        <v>0.04005769306222779</v>
+        <v>0.04005769306163229</v>
       </c>
       <c r="E22" t="n">
-        <v>4.52966622438198e-06</v>
+        <v>4.529666224281081e-06</v>
       </c>
       <c r="F22" t="n">
-        <v>4.363449440804301e-05</v>
+        <v>4.363449440610012e-05</v>
       </c>
       <c r="G22" t="n">
-        <v>5.769306193915275e-05</v>
+        <v>5.769306193659229e-05</v>
       </c>
     </row>
     <row r="23">
@@ -1570,19 +1570,19 @@
         <v>22</v>
       </c>
       <c r="C23" t="n">
-        <v>0.9396127564086452</v>
+        <v>0.9396127566140287</v>
       </c>
       <c r="D23" t="n">
-        <v>0.457243045398621</v>
+        <v>0.4572430448510221</v>
       </c>
       <c r="E23" t="n">
-        <v>4.848238130652082e-05</v>
+        <v>4.848238129618112e-05</v>
       </c>
       <c r="F23" t="n">
-        <v>0.003181629066287606</v>
+        <v>0.003181629064930469</v>
       </c>
       <c r="G23" t="n">
-        <v>0.002173972165639415</v>
+        <v>0.002173972164712046</v>
       </c>
     </row>
     <row r="24">
@@ -1593,19 +1593,19 @@
         <v>23</v>
       </c>
       <c r="C24" t="n">
-        <v>0.8464311272560053</v>
+        <v>0.8464311276633153</v>
       </c>
       <c r="D24" t="n">
-        <v>0.4050690733675816</v>
+        <v>0.405069072661614</v>
       </c>
       <c r="E24" t="n">
-        <v>4.369606441686406e-05</v>
+        <v>4.36960644126869e-05</v>
       </c>
       <c r="F24" t="n">
-        <v>0.005143675371587775</v>
+        <v>0.005143675370604339</v>
       </c>
       <c r="G24" t="n">
-        <v>0.004061670608009826</v>
+        <v>0.004061670607233281</v>
       </c>
     </row>
     <row r="25">
@@ -1616,19 +1616,19 @@
         <v>24</v>
       </c>
       <c r="C25" t="n">
-        <v>0.4212874520481766</v>
+        <v>0.4212874523514668</v>
       </c>
       <c r="D25" t="n">
-        <v>0.2010074027637769</v>
+        <v>0.2010074022802691</v>
       </c>
       <c r="E25" t="n">
-        <v>2.188544011398888e-05</v>
+        <v>2.188544011343908e-05</v>
       </c>
       <c r="F25" t="n">
-        <v>0.001287452300954117</v>
+        <v>0.001287452300889336</v>
       </c>
       <c r="G25" t="n">
-        <v>0.001007402687721981</v>
+        <v>0.001007402687671355</v>
       </c>
     </row>
     <row r="26">
@@ -1639,19 +1639,19 @@
         <v>25</v>
       </c>
       <c r="C26" t="n">
-        <v>0.9507797474183275</v>
+        <v>0.9507797337046475</v>
       </c>
       <c r="D26" t="n">
-        <v>0.9736359369623292</v>
+        <v>0.9736358987349264</v>
       </c>
       <c r="E26" t="n">
-        <v>6.535174917750251e-05</v>
+        <v>6.535174736330369e-05</v>
       </c>
       <c r="F26" t="n">
-        <v>0.002600896313714074</v>
+        <v>0.002600896169309586</v>
       </c>
       <c r="G26" t="n">
-        <v>0.00132479152136955</v>
+        <v>0.001324791447815832</v>
       </c>
     </row>
     <row r="27">
@@ -1662,19 +1662,19 @@
         <v>26</v>
       </c>
       <c r="C27" t="n">
-        <v>0.8881788532567664</v>
+        <v>0.8881788420489906</v>
       </c>
       <c r="D27" t="n">
-        <v>0.9473111431062776</v>
+        <v>0.9473111032797028</v>
       </c>
       <c r="E27" t="n">
-        <v>6.248678200541497e-05</v>
+        <v>6.248678019649359e-05</v>
       </c>
       <c r="F27" t="n">
-        <v>0.003328993610318354</v>
+        <v>0.003328993417577308</v>
       </c>
       <c r="G27" t="n">
-        <v>0.001694952059863031</v>
+        <v>0.001694951961728974</v>
       </c>
     </row>
     <row r="28">
@@ -1685,19 +1685,19 @@
         <v>27</v>
       </c>
       <c r="C28" t="n">
-        <v>0.8248498569898606</v>
+        <v>0.8248498630071616</v>
       </c>
       <c r="D28" t="n">
-        <v>0.9206162022974929</v>
+        <v>0.9206161581942242</v>
       </c>
       <c r="E28" t="n">
-        <v>5.964189029827223e-05</v>
+        <v>5.96418888631227e-05</v>
       </c>
       <c r="F28" t="n">
-        <v>0.01130085566341799</v>
+        <v>0.01130085511955781</v>
       </c>
       <c r="G28" t="n">
-        <v>0.009963747812023804</v>
+        <v>0.009963747332513151</v>
       </c>
     </row>
     <row r="29">
@@ -1708,19 +1708,19 @@
         <v>28</v>
       </c>
       <c r="C29" t="n">
-        <v>0.7535490080901626</v>
+        <v>0.7535490334342411</v>
       </c>
       <c r="D29" t="n">
-        <v>0.8906524483912845</v>
+        <v>0.8906523938463247</v>
       </c>
       <c r="E29" t="n">
-        <v>5.698170403144277e-05</v>
+        <v>5.698170274011765e-05</v>
       </c>
       <c r="F29" t="n">
-        <v>0.007833349480933505</v>
+        <v>0.007833349125893174</v>
       </c>
       <c r="G29" t="n">
-        <v>0.006824228607736904</v>
+        <v>0.006824228298434099</v>
       </c>
     </row>
     <row r="30">
@@ -1731,19 +1731,19 @@
         <v>29</v>
       </c>
       <c r="C30" t="n">
-        <v>0.6257156770718593</v>
+        <v>0.6257156960292669</v>
       </c>
       <c r="D30" t="n">
-        <v>0.8138281853306817</v>
+        <v>0.813828129340177</v>
       </c>
       <c r="E30" t="n">
-        <v>5.05844088793934e-05</v>
+        <v>5.058440720353237e-05</v>
       </c>
       <c r="F30" t="n">
-        <v>0.003895668322469015</v>
+        <v>0.003895668064342273</v>
       </c>
       <c r="G30" t="n">
-        <v>0.001984296081494086</v>
+        <v>0.001984295950014814</v>
       </c>
     </row>
     <row r="31">
@@ -1754,19 +1754,19 @@
         <v>30</v>
       </c>
       <c r="C31" t="n">
-        <v>0.4218199765318016</v>
+        <v>0.4218200046048902</v>
       </c>
       <c r="D31" t="n">
-        <v>0.211843963924265</v>
+        <v>0.2118439316951737</v>
       </c>
       <c r="E31" t="n">
-        <v>2.334908741850188e-05</v>
+        <v>2.334908791615493e-05</v>
       </c>
       <c r="F31" t="n">
-        <v>0.001593637961557537</v>
+        <v>0.001593638029489919</v>
       </c>
       <c r="G31" t="n">
-        <v>0.001574993182450635</v>
+        <v>0.00157499324958818</v>
       </c>
     </row>
     <row r="32">
@@ -1777,19 +1777,19 @@
         <v>31</v>
       </c>
       <c r="C32" t="n">
-        <v>0.2702263433429942</v>
+        <v>0.2702263664708566</v>
       </c>
       <c r="D32" t="n">
-        <v>0.1402689702359918</v>
+        <v>0.1402689478371155</v>
       </c>
       <c r="E32" t="n">
-        <v>1.51286996633696e-05</v>
+        <v>1.512870015198995e-05</v>
       </c>
       <c r="F32" t="n">
-        <v>0.0002131951771218721</v>
+        <v>0.000213195190893245</v>
       </c>
       <c r="G32" t="n">
-        <v>0.0002484873900174267</v>
+        <v>0.0002484874060685316</v>
       </c>
     </row>
     <row r="33">
@@ -1800,19 +1800,19 @@
         <v>32</v>
       </c>
       <c r="C33" t="n">
-        <v>0.06001316318190804</v>
+        <v>0.06001316970401727</v>
       </c>
       <c r="D33" t="n">
-        <v>0.04002047651485117</v>
+        <v>0.04002047175196148</v>
       </c>
       <c r="E33" t="n">
-        <v>3.587869413815667e-06</v>
+        <v>3.587869547831241e-06</v>
       </c>
       <c r="F33" t="n">
-        <v>1.31686181136792e-05</v>
+        <v>1.316861909745476e-05</v>
       </c>
       <c r="G33" t="n">
-        <v>2.047507719611652e-05</v>
+        <v>2.047507872571241e-05</v>
       </c>
     </row>
     <row r="34">
@@ -1988,7 +1988,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.2026771169693317</v>
+        <v>0.2026771126692801</v>
       </c>
     </row>
     <row r="5">
@@ -1998,7 +1998,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>5.455642448703411</v>
+        <v>5.455642332955049</v>
       </c>
     </row>
   </sheetData>

</xml_diff>